<commit_message>
Logica de Camiones + Carga en pala
</commit_message>
<xml_diff>
--- a/Informacion Palas.xlsx
+++ b/Informacion Palas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Collahuasi-Validador-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8AB258-5BD1-4EA9-BC85-210B94407A06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AAA244-FBDC-4F2F-A467-7A5E90F9AAB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CS03" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -598,7 +598,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="A2:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1017,13 +1017,13 @@
         <v>0.32</v>
       </c>
       <c r="F2" s="4">
-        <v>82</v>
+        <v>1.3666666666666667</v>
       </c>
       <c r="G2" s="4">
-        <v>102</v>
+        <v>1.7</v>
       </c>
       <c r="H2" s="4">
-        <v>122</v>
+        <v>2.0333333333333332</v>
       </c>
       <c r="I2" s="4">
         <f>70/60</f>
@@ -1032,7 +1032,6 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G3" s="1"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1105,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1168,13 +1167,13 @@
         <v>0.08</v>
       </c>
       <c r="F2">
-        <v>40.020000000000003</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="G2">
-        <v>88.714285714285694</v>
+        <v>1.4785714285714282</v>
       </c>
       <c r="H2">
-        <v>161.69433962264199</v>
+        <v>2.6949056603773665</v>
       </c>
       <c r="I2">
         <f>70/60</f>
@@ -1201,13 +1200,13 @@
         <v>0.04</v>
       </c>
       <c r="F3">
-        <v>43.251428571428598</v>
+        <v>0.72085714285714331</v>
       </c>
       <c r="G3">
-        <v>88.714285714285694</v>
+        <v>1.4785714285714282</v>
       </c>
       <c r="H3">
-        <v>148.98367346938801</v>
+        <v>2.4830612244898003</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I14" si="0">70/60</f>
@@ -1234,13 +1233,13 @@
         <v>0.1</v>
       </c>
       <c r="F4">
-        <v>43.981671606401903</v>
+        <v>0.7330278601066984</v>
       </c>
       <c r="G4">
-        <v>88.714285714285694</v>
+        <v>1.4785714285714282</v>
       </c>
       <c r="H4">
-        <v>149.01311688311699</v>
+        <v>2.4835519480519497</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -1267,13 +1266,13 @@
         <v>0.12</v>
       </c>
       <c r="F5">
-        <v>146.53848942598199</v>
+        <v>2.4423081570997001</v>
       </c>
       <c r="G5">
-        <v>276</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H5">
-        <v>470.06442953020098</v>
+        <v>7.834407158836683</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
@@ -1300,13 +1299,13 @@
         <v>0.08</v>
       </c>
       <c r="F6">
-        <v>62.8314000157078</v>
+        <v>1.0471900002617966</v>
       </c>
       <c r="G6">
-        <v>108.33000002708199</v>
+        <v>1.8055000004513666</v>
       </c>
       <c r="H6">
-        <v>174.848421096344</v>
+        <v>2.9141403516057331</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
@@ -1333,13 +1332,13 @@
         <v>0.1</v>
       </c>
       <c r="F7">
-        <v>51.561193734863402</v>
+        <v>0.85935322891439003</v>
       </c>
       <c r="G7">
-        <v>108.33000002708199</v>
+        <v>1.8055000004513666</v>
       </c>
       <c r="H7">
-        <v>180.397587707437</v>
+        <v>3.0066264617906167</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -1366,13 +1365,13 @@
         <v>0.02</v>
       </c>
       <c r="F8">
-        <v>52.193279378127698</v>
+        <v>0.86988798963546166</v>
       </c>
       <c r="G8">
-        <v>108.33000002708199</v>
+        <v>1.8055000004513666</v>
       </c>
       <c r="H8">
-        <v>179.73683592279701</v>
+        <v>2.9956139320466169</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
@@ -1399,13 +1398,13 @@
         <v>0.18</v>
       </c>
       <c r="F9">
-        <v>57.268203139317002</v>
+        <v>0.95447005232195004</v>
       </c>
       <c r="G9">
-        <v>108.33000002708199</v>
+        <v>1.8055000004513666</v>
       </c>
       <c r="H9">
-        <v>176.52593362346701</v>
+        <v>2.9420988937244501</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
@@ -1432,13 +1431,13 @@
         <v>0.08</v>
       </c>
       <c r="F10">
-        <v>47.183376623376603</v>
+        <v>0.78638961038961008</v>
       </c>
       <c r="G10">
-        <v>88.714285714285694</v>
+        <v>1.4785714285714282</v>
       </c>
       <c r="H10">
-        <v>151.83189075630301</v>
+        <v>2.5305315126050503</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
@@ -1465,13 +1464,13 @@
         <v>0.22</v>
       </c>
       <c r="F11">
-        <v>54.830014200511201</v>
+        <v>0.91383357000852006</v>
       </c>
       <c r="G11">
-        <v>88.714285714285694</v>
+        <v>1.4785714285714282</v>
       </c>
       <c r="H11">
-        <v>135.40047116471899</v>
+        <v>2.256674519411983</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
@@ -1498,13 +1497,13 @@
         <v>0.08</v>
       </c>
       <c r="F12">
-        <v>51.063493670886103</v>
+        <v>0.8510582278481017</v>
       </c>
       <c r="G12">
-        <v>88.714285714285694</v>
+        <v>1.4785714285714282</v>
       </c>
       <c r="H12">
-        <v>148.156118697479</v>
+        <v>2.4692686449579835</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
@@ -1531,13 +1530,13 @@
         <v>0.24</v>
       </c>
       <c r="F13">
-        <v>258.22904998881</v>
+        <v>4.3038174998135004</v>
       </c>
       <c r="G13">
-        <v>368.459999984033</v>
+        <v>6.1409999997338831</v>
       </c>
       <c r="H13">
-        <v>552.18982803036999</v>
+        <v>9.2031638005061662</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
@@ -1564,13 +1563,13 @@
         <v>0.02</v>
       </c>
       <c r="F14">
-        <v>280.21959777791199</v>
+        <v>4.6703266296318668</v>
       </c>
       <c r="G14">
-        <v>368.459999984033</v>
+        <v>6.1409999997338831</v>
       </c>
       <c r="H14">
-        <v>530.14941702771796</v>
+        <v>8.8358236171286322</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Comienzo test dinamico dispatch
</commit_message>
<xml_diff>
--- a/Informacion Palas.xlsx
+++ b/Informacion Palas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Collahuasi-Validador-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8A7A1E-6153-4D58-939A-F956690B3A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26EF3D9-472C-43FE-A0BD-C509AF1441AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>NP</t>
   </si>
@@ -108,13 +108,29 @@
   </si>
   <si>
     <t>Media Recuperacion (Exponencial) / min</t>
+  </si>
+  <si>
+    <t>PA09</t>
+  </si>
+  <si>
+    <t>CF05</t>
+  </si>
+  <si>
+    <t>CF06</t>
+  </si>
+  <si>
+    <t>PA06</t>
+  </si>
+  <si>
+    <t>PA08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
@@ -253,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,8 +449,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -549,8 +571,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -593,15 +626,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -629,6 +664,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="42" builtinId="6"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1103,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A2:A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,8 +1188,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B2">
         <v>272.23224900000002</v>
@@ -1185,8 +1221,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B3">
         <v>303.81824999999998</v>
@@ -1210,7 +1246,7 @@
         <v>2.4830612244898003</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I14" si="0">70/60</f>
+        <f t="shared" ref="I3:I9" si="0">70/60</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="J3">
@@ -1218,8 +1254,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="B4">
         <v>561.91379640000002</v>
@@ -1251,8 +1287,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B5">
         <v>182.04741540000001</v>
@@ -1284,8 +1320,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B6">
         <v>236.96753819999998</v>
@@ -1317,7 +1353,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7">
@@ -1350,8 +1386,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
+      <c r="A8" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B8">
         <v>295.42289099999999</v>
@@ -1383,8 +1419,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="A9" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="B9">
         <v>250.71384959999997</v>
@@ -1416,169 +1452,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>272.23224900000002</v>
-      </c>
-      <c r="C10">
-        <v>21.4404696</v>
-      </c>
-      <c r="D10">
-        <v>0.06</v>
-      </c>
-      <c r="E10">
-        <v>0.08</v>
-      </c>
-      <c r="F10">
-        <v>0.78638961038961008</v>
-      </c>
-      <c r="G10">
-        <v>1.4785714285714282</v>
-      </c>
-      <c r="H10">
-        <v>2.5305315126050503</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J10">
-        <v>9970</v>
-      </c>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>267.7259052</v>
-      </c>
-      <c r="C11">
-        <v>49.274788199999996</v>
-      </c>
-      <c r="D11">
-        <v>0.2</v>
-      </c>
-      <c r="E11">
-        <v>0.22</v>
-      </c>
-      <c r="F11">
-        <v>0.91383357000852006</v>
-      </c>
-      <c r="G11">
-        <v>1.4785714285714282</v>
-      </c>
-      <c r="H11">
-        <v>2.256674519411983</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J11">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>250.07163300000002</v>
-      </c>
-      <c r="C12">
-        <v>34.7467392</v>
-      </c>
-      <c r="D12">
-        <v>0.08</v>
-      </c>
-      <c r="E12">
-        <v>0.08</v>
-      </c>
-      <c r="F12">
-        <v>0.8510582278481017</v>
-      </c>
-      <c r="G12">
-        <v>1.4785714285714282</v>
-      </c>
-      <c r="H12">
-        <v>2.4692686449579835</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J12">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>262.8486714</v>
-      </c>
-      <c r="C13">
-        <v>39.323863799999998</v>
-      </c>
-      <c r="D13">
-        <v>1.5</v>
-      </c>
-      <c r="E13">
-        <v>0.24</v>
-      </c>
-      <c r="F13">
-        <v>4.3038174998135004</v>
-      </c>
-      <c r="G13">
-        <v>6.1409999997338831</v>
-      </c>
-      <c r="H13">
-        <v>9.2031638005061662</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J13">
-        <v>2931</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>285.87496379999999</v>
-      </c>
-      <c r="C14">
-        <v>24.5580912</v>
-      </c>
-      <c r="D14">
-        <v>1.5</v>
-      </c>
-      <c r="E14">
-        <v>0.02</v>
-      </c>
-      <c r="F14">
-        <v>4.6703266296318668</v>
-      </c>
-      <c r="G14">
-        <v>6.1409999997338831</v>
-      </c>
-      <c r="H14">
-        <v>8.8358236171286322</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J14">
-        <v>2931</v>
-      </c>
+      <c r="A11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Regresion Lineal para estimar tiempos
</commit_message>
<xml_diff>
--- a/Informacion Palas.xlsx
+++ b/Informacion Palas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Collahuasi-Validador-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D45AD97-7A1D-45BB-93C2-01174A2EE741}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA556281-1F5F-4311-9EF1-4B0DBCF45711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CS03" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>NP</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Media Recuperacion (Exponencial) / min</t>
+  </si>
+  <si>
+    <t>PAA</t>
+  </si>
+  <si>
+    <t>PAB</t>
+  </si>
+  <si>
+    <t>PAC</t>
+  </si>
+  <si>
+    <t>PAD</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1153,7 +1165,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>272.23224900000002</v>
@@ -1186,7 +1198,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>303.81824999999998</v>
@@ -1210,7 +1222,7 @@
         <v>2.4830612244898003</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="0">70/60</f>
+        <f t="shared" ref="I3:I5" si="0">70/60</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="J3">
@@ -1219,7 +1231,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>561.91379640000002</v>
@@ -1252,7 +1264,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>182.04741540000001</v>
@@ -1281,204 +1293,6 @@
       </c>
       <c r="J5">
         <v>3913</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>236.96753819999998</v>
-      </c>
-      <c r="C6">
-        <v>22.7830206</v>
-      </c>
-      <c r="D6">
-        <v>0.08</v>
-      </c>
-      <c r="E6">
-        <v>0.08</v>
-      </c>
-      <c r="F6">
-        <v>1.0471900002617966</v>
-      </c>
-      <c r="G6">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="H6">
-        <v>2.9141403516057331</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J6">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>233.01076860000001</v>
-      </c>
-      <c r="C7">
-        <v>16.598233200000003</v>
-      </c>
-      <c r="D7">
-        <v>0.08</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7">
-        <v>0.85935322891439003</v>
-      </c>
-      <c r="G7">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="H7">
-        <v>3.0066264617906167</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J7">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>295.42289099999999</v>
-      </c>
-      <c r="C8">
-        <v>12.1300092</v>
-      </c>
-      <c r="D8">
-        <v>0.02</v>
-      </c>
-      <c r="E8">
-        <v>0.02</v>
-      </c>
-      <c r="F8">
-        <v>0.86988798963546166</v>
-      </c>
-      <c r="G8">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="H8">
-        <v>2.9956139320466169</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J8">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>250.71384959999997</v>
-      </c>
-      <c r="C9">
-        <v>18.368355600000001</v>
-      </c>
-      <c r="D9">
-        <v>0.18</v>
-      </c>
-      <c r="E9">
-        <v>0.18</v>
-      </c>
-      <c r="F9">
-        <v>0.95447005232195004</v>
-      </c>
-      <c r="G9">
-        <v>1.8055000004513666</v>
-      </c>
-      <c r="H9">
-        <v>2.9420988937244501</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J9">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>272.23224900000002</v>
-      </c>
-      <c r="C10">
-        <v>21.4404696</v>
-      </c>
-      <c r="D10">
-        <v>0.06</v>
-      </c>
-      <c r="E10">
-        <v>0.08</v>
-      </c>
-      <c r="F10">
-        <v>0.78638961038961008</v>
-      </c>
-      <c r="G10">
-        <v>1.4785714285714282</v>
-      </c>
-      <c r="H10">
-        <v>2.5305315126050503</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J10">
-        <v>9970</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>267.7259052</v>
-      </c>
-      <c r="C11">
-        <v>49.274788199999996</v>
-      </c>
-      <c r="D11">
-        <v>0.2</v>
-      </c>
-      <c r="E11">
-        <v>0.22</v>
-      </c>
-      <c r="F11">
-        <v>0.91383357000852006</v>
-      </c>
-      <c r="G11">
-        <v>1.4785714285714282</v>
-      </c>
-      <c r="H11">
-        <v>2.256674519411983</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="J11">
-        <v>9970</v>
       </c>
     </row>
   </sheetData>
@@ -1488,14 +1302,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F995BFD6-B4AF-48CC-8B8C-8697BD459696}">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Revision de extraccion en curso
</commit_message>
<xml_diff>
--- a/Informacion Palas.xlsx
+++ b/Informacion Palas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Collahuasi-Validador-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA556281-1F5F-4311-9EF1-4B0DBCF45711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A17D8FB-1636-4D03-8C67-B4A43448EFD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CS03" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>NP</t>
   </si>
@@ -108,18 +108,6 @@
   </si>
   <si>
     <t>Media Recuperacion (Exponencial) / min</t>
-  </si>
-  <si>
-    <t>PAA</t>
-  </si>
-  <si>
-    <t>PAB</t>
-  </si>
-  <si>
-    <t>PAC</t>
-  </si>
-  <si>
-    <t>PAD</t>
   </si>
 </sst>
 </file>
@@ -1115,21 +1103,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="3" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" customWidth="1"/>
-    <col min="7" max="7" width="24.90625" customWidth="1"/>
-    <col min="8" max="8" width="20.90625" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1165,7 +1145,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>272.23224900000002</v>
@@ -1198,7 +1178,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>303.81824999999998</v>
@@ -1222,7 +1202,7 @@
         <v>2.4830612244898003</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I5" si="0">70/60</f>
+        <f t="shared" ref="I3:I11" si="0">70/60</f>
         <v>1.1666666666666667</v>
       </c>
       <c r="J3">
@@ -1231,7 +1211,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>561.91379640000002</v>
@@ -1264,7 +1244,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>182.04741540000001</v>
@@ -1293,6 +1273,204 @@
       </c>
       <c r="J5">
         <v>3913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>236.96753819999998</v>
+      </c>
+      <c r="C6">
+        <v>22.7830206</v>
+      </c>
+      <c r="D6">
+        <v>0.08</v>
+      </c>
+      <c r="E6">
+        <v>0.08</v>
+      </c>
+      <c r="F6">
+        <v>1.0471900002617966</v>
+      </c>
+      <c r="G6">
+        <v>1.8055000004513666</v>
+      </c>
+      <c r="H6">
+        <v>2.9141403516057331</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J6">
+        <v>9970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>233.01076860000001</v>
+      </c>
+      <c r="C7">
+        <v>16.598233200000003</v>
+      </c>
+      <c r="D7">
+        <v>0.08</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>0.85935322891439003</v>
+      </c>
+      <c r="G7">
+        <v>1.8055000004513666</v>
+      </c>
+      <c r="H7">
+        <v>3.0066264617906167</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J7">
+        <v>9970</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>295.42289099999999</v>
+      </c>
+      <c r="C8">
+        <v>12.1300092</v>
+      </c>
+      <c r="D8">
+        <v>0.02</v>
+      </c>
+      <c r="E8">
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>0.86988798963546166</v>
+      </c>
+      <c r="G8">
+        <v>1.8055000004513666</v>
+      </c>
+      <c r="H8">
+        <v>2.9956139320466169</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J8">
+        <v>9970</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>250.71384959999997</v>
+      </c>
+      <c r="C9">
+        <v>18.368355600000001</v>
+      </c>
+      <c r="D9">
+        <v>0.18</v>
+      </c>
+      <c r="E9">
+        <v>0.18</v>
+      </c>
+      <c r="F9">
+        <v>0.95447005232195004</v>
+      </c>
+      <c r="G9">
+        <v>1.8055000004513666</v>
+      </c>
+      <c r="H9">
+        <v>2.9420988937244501</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J9">
+        <v>9970</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>262.8486714</v>
+      </c>
+      <c r="C10">
+        <v>39.323863799999998</v>
+      </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="E10">
+        <v>0.24</v>
+      </c>
+      <c r="F10">
+        <v>4.3038174998135004</v>
+      </c>
+      <c r="G10">
+        <v>6.1409999997338831</v>
+      </c>
+      <c r="H10">
+        <v>9.2031638005061662</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J10">
+        <v>2931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>285.87496379999999</v>
+      </c>
+      <c r="C11">
+        <v>24.5580912</v>
+      </c>
+      <c r="D11">
+        <v>1.5</v>
+      </c>
+      <c r="E11">
+        <v>0.02</v>
+      </c>
+      <c r="F11">
+        <v>4.6703266296318668</v>
+      </c>
+      <c r="G11">
+        <v>6.1409999997338831</v>
+      </c>
+      <c r="H11">
+        <v>8.8358236171286322</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="J11">
+        <v>2931</v>
       </c>
     </row>
   </sheetData>
@@ -1304,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F995BFD6-B4AF-48CC-8B8C-8697BD459696}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>